<commit_message>
finally, the real deal
</commit_message>
<xml_diff>
--- a/incomestatementformat.xlsx
+++ b/incomestatementformat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianbaime/Desktop/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73601CA-98C8-D641-92A8-21E8C87CB585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83D6286-80EE-3949-9E9A-B7EAD0BF671D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{BF3D2BD5-3565-4B0B-8265-0C0C1F0B094C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{BF3D2BD5-3565-4B0B-8265-0C0C1F0B094C}"/>
   </bookViews>
   <sheets>
     <sheet name="Income Statement" sheetId="3" r:id="rId1"/>
@@ -57,25 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">© Corporate Finance Institute. All rights reserved.  </t>
-  </si>
-  <si>
-    <t>Historical --&gt;</t>
-  </si>
-  <si>
-    <t>Forecast --&gt;</t>
-  </si>
-  <si>
-    <t>3 Statement Model</t>
-  </si>
-  <si>
-    <t>USD millions, except per share data</t>
-  </si>
-  <si>
-    <t>Income Statement</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Revenues</t>
   </si>
@@ -86,9 +68,6 @@
     <t>Net Income</t>
   </si>
   <si>
-    <t>Base Year</t>
-  </si>
-  <si>
     <t>Year 1</t>
   </si>
   <si>
@@ -123,20 +102,22 @@
   </si>
   <si>
     <t>EBIT</t>
+  </si>
+  <si>
+    <t>5 Year P&amp;L Projection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\(#,##0\)_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0&quot;A&quot;"/>
-    <numFmt numFmtId="167" formatCode="0&quot;E&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0_);\(#,##0\);\-"/>
+    <numFmt numFmtId="166" formatCode="0&quot;E&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0_);\(#,##0\);\-"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -150,60 +131,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="0"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Bookman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -212,8 +142,50 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,24 +194,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF132E57"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1E8496"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED942D"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -256,62 +222,36 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="37" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="37" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="37" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{7B55658A-63F6-4A23-9179-88B5E6431BBC}"/>
@@ -655,149 +595,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1485A874-E043-FA40-A16F-2EBFA932A537}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="14">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="16">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="18">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" ht="18">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18">
-      <c r="A4" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="14">
-      <c r="A5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" ht="14">
-      <c r="A6" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="14">
-      <c r="A7" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="14">
-      <c r="A8" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="14">
-      <c r="A9" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="14">
-      <c r="A10" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14">
-      <c r="A11" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="14">
-      <c r="A12" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14">
-      <c r="A13" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14">
-      <c r="A14" s="14" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="15">
+      <c r="A5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" ht="15">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="14">
-      <c r="A15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1">
-      <c r="A16" s="15"/>
-    </row>
-    <row r="17" spans="1:1" ht="15" thickTop="1">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:1" ht="14">
-      <c r="A18" s="12"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="15">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" ht="15">
+      <c r="A8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="15">
+      <c r="A9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="15">
+      <c r="A10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="15">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="15">
+      <c r="A12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="14">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3">
+  <conditionalFormatting sqref="A1">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",A3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OK",A1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",A3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ERROR",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>